<commit_message>
Fiordland and Patagonia analyses
</commit_message>
<xml_diff>
--- a/Aggregated/ELA_estimates.xlsx
+++ b/Aggregated/ELA_estimates.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/colinstark/Science/slm_glacial_srtm/Aggregated/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/colinstark/Science/slmGlacial/slmGlacialSRTM/master/Aggregated/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="15020" yWindow="8420" windowWidth="23380" windowHeight="15280"/>
+    <workbookView xWindow="6160" yWindow="4080" windowWidth="15260" windowHeight="11180"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Cascades_ROI1</t>
   </si>
@@ -75,6 +75,12 @@
   </si>
   <si>
     <t>SouthernAlpsNZ_ROI3</t>
+  </si>
+  <si>
+    <t>FiordlandNZ_ROI1</t>
+  </si>
+  <si>
+    <t>Patagonia_ROI1</t>
   </si>
 </sst>
 </file>
@@ -441,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -493,10 +499,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="C4">
-        <v>4000</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -504,7 +510,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C5">
         <v>4000</v>
@@ -515,7 +521,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C6">
         <v>4000</v>
@@ -526,42 +532,40 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C7">
-        <v>3800</v>
+        <v>500</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C8">
-        <v>600</v>
-      </c>
-      <c r="E8" s="1"/>
+        <v>4000</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C9">
-        <v>600</v>
-      </c>
-      <c r="E9" s="1"/>
+        <v>3800</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C10">
         <v>600</v>
@@ -570,34 +574,58 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C11">
-        <v>3500</v>
-      </c>
+        <v>600</v>
+      </c>
+      <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="C12">
-        <v>2650</v>
-      </c>
+        <v>600</v>
+      </c>
+      <c r="E12" s="1"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13">
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14">
         <v>12</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14">
+        <v>2650</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C13">
+      <c r="C15">
         <v>2200</v>
       </c>
     </row>

</xml_diff>